<commit_message>
+ Prototype is finished
</commit_message>
<xml_diff>
--- a/src/lakersquiz.xlsx
+++ b/src/lakersquiz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\Programming Projects\minor-projects\javascript-areyouatruelakersfan\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\Programming Projects\javascript-areyouatruelakersfan\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A30687-5EE7-4498-BE4D-80B560DDEE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D94AF3-D166-4B0E-91D8-C56593A1A46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,12 +46,6 @@
     <t>What's Lebron's Nickname?</t>
   </si>
   <si>
-    <t>LBJ</t>
-  </si>
-  <si>
-    <t>The Queen;LeGM;LeCoach</t>
-  </si>
-  <si>
     <t>Who's AD?</t>
   </si>
   <si>
@@ -73,18 +67,12 @@
     <t>What date did Alex Caruso sign with Oklahoma City Thunder?</t>
   </si>
   <si>
-    <t>Donation for Lakers G-League team; Donation to Repulican Party;Donation for Democratic Party</t>
-  </si>
-  <si>
     <t>Why did Alex Caruso shave his head (Hint: Awareness)?</t>
   </si>
   <si>
     <t>Which Player was the most google searched on 3/16/2022?</t>
   </si>
   <si>
-    <t>Not Ready;Not Ready;Not Ready</t>
-  </si>
-  <si>
     <t>Lebron James</t>
   </si>
   <si>
@@ -94,9 +82,6 @@
     <t>Donation for testicular cancer research</t>
   </si>
   <si>
-    <t>Donation to his former school (A&amp;M Consolidated High School); Donation to Repulican Party;Donation for Democratic Party</t>
-  </si>
-  <si>
     <t>Natalia Bryant</t>
   </si>
   <si>
@@ -142,9 +127,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Yes;Yes;Yes</t>
-  </si>
-  <si>
     <t>What was the offensive rating of 2002-03 Lakers team during regular season?</t>
   </si>
   <si>
@@ -236,6 +218,24 @@
   </si>
   <si>
     <t>7/11/2014;7/12/2014;7/14/2014</t>
+  </si>
+  <si>
+    <t>Donation to his former school; Donation to Church for Tax Deductible;Donation for Democratic Party</t>
+  </si>
+  <si>
+    <t>Frank Thompson;Roland Dore;Andrew Brook</t>
+  </si>
+  <si>
+    <t>No;No;No</t>
+  </si>
+  <si>
+    <t>8/16/2015;11/13/2016;1/13/2017</t>
+  </si>
+  <si>
+    <t>The King</t>
+  </si>
+  <si>
+    <t>The Queen;The Qing;Black Mamba</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,10 +1139,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1150,13 +1150,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1164,13 +1164,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1178,13 +1178,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,13 +1192,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2">
         <v>42636</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1206,13 +1206,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1220,13 +1220,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1234,13 +1234,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,13 +1248,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>42459</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,13 +1262,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,13 +1276,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,13 +1290,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1304,13 +1304,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1318,13 +1318,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1">
         <v>107.2</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,13 +1332,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,13 +1346,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,13 +1360,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,13 +1374,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1">
         <v>150</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,13 +1388,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3">
         <v>0.13</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,13 +1402,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,13 +1416,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,13 +1430,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,13 +1444,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,13 +1458,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1">
         <v>2010</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,13 +1472,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2">
         <v>41833</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>